<commit_message>
Added main_scores and weights
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,16 @@
           <t>sentence</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>main_score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -468,6 +478,12 @@
 </t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>40</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5336644649505615</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -487,6 +503,12 @@
 </t>
         </is>
       </c>
+      <c r="E3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.5336644649505615</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -506,6 +528,12 @@
 </t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>40</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.5336644649505615</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -525,6 +553,12 @@
 </t>
         </is>
       </c>
+      <c r="E5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.5336644649505615</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -544,6 +578,12 @@
 </t>
         </is>
       </c>
+      <c r="E6" t="n">
+        <v>40</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5336644649505615</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -563,6 +603,12 @@
 </t>
         </is>
       </c>
+      <c r="E7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.5336644649505615</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -582,6 +628,12 @@
 </t>
         </is>
       </c>
+      <c r="E8" t="n">
+        <v>40</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.5336644649505615</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -603,6 +655,12 @@
 </t>
         </is>
       </c>
+      <c r="E9" t="n">
+        <v>40</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -624,6 +682,12 @@
 </t>
         </is>
       </c>
+      <c r="E10" t="n">
+        <v>40</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -645,6 +709,12 @@
 </t>
         </is>
       </c>
+      <c r="E11" t="n">
+        <v>40</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -666,6 +736,12 @@
 </t>
         </is>
       </c>
+      <c r="E12" t="n">
+        <v>40</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -687,6 +763,12 @@
 </t>
         </is>
       </c>
+      <c r="E13" t="n">
+        <v>40</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -708,6 +790,12 @@
 </t>
         </is>
       </c>
+      <c r="E14" t="n">
+        <v>40</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -729,6 +817,12 @@
 </t>
         </is>
       </c>
+      <c r="E15" t="n">
+        <v>40</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -750,6 +844,12 @@
 </t>
         </is>
       </c>
+      <c r="E16" t="n">
+        <v>40</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -771,6 +871,12 @@
 </t>
         </is>
       </c>
+      <c r="E17" t="n">
+        <v>40</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -792,6 +898,12 @@
 </t>
         </is>
       </c>
+      <c r="E18" t="n">
+        <v>40</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.4905979931354523</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -812,6 +924,12 @@
 </t>
         </is>
       </c>
+      <c r="E19" t="n">
+        <v>40</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -832,6 +950,12 @@
 </t>
         </is>
       </c>
+      <c r="E20" t="n">
+        <v>40</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -852,6 +976,12 @@
 </t>
         </is>
       </c>
+      <c r="E21" t="n">
+        <v>40</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -872,6 +1002,12 @@
 </t>
         </is>
       </c>
+      <c r="E22" t="n">
+        <v>40</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -892,6 +1028,12 @@
 </t>
         </is>
       </c>
+      <c r="E23" t="n">
+        <v>40</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -912,6 +1054,12 @@
 </t>
         </is>
       </c>
+      <c r="E24" t="n">
+        <v>40</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -932,6 +1080,12 @@
 </t>
         </is>
       </c>
+      <c r="E25" t="n">
+        <v>40</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -952,6 +1106,12 @@
 </t>
         </is>
       </c>
+      <c r="E26" t="n">
+        <v>40</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -972,6 +1132,12 @@
 </t>
         </is>
       </c>
+      <c r="E27" t="n">
+        <v>40</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -992,6 +1158,12 @@
 </t>
         </is>
       </c>
+      <c r="E28" t="n">
+        <v>40</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1012,6 +1184,12 @@
 </t>
         </is>
       </c>
+      <c r="E29" t="n">
+        <v>40</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1032,6 +1210,12 @@
 </t>
         </is>
       </c>
+      <c r="E30" t="n">
+        <v>40</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1052,6 +1236,12 @@
 </t>
         </is>
       </c>
+      <c r="E31" t="n">
+        <v>40</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1072,6 +1262,12 @@
 </t>
         </is>
       </c>
+      <c r="E32" t="n">
+        <v>40</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1092,6 +1288,12 @@
 </t>
         </is>
       </c>
+      <c r="E33" t="n">
+        <v>40</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1112,6 +1314,12 @@
 </t>
         </is>
       </c>
+      <c r="E34" t="n">
+        <v>40</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1132,6 +1340,12 @@
 </t>
         </is>
       </c>
+      <c r="E35" t="n">
+        <v>40</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1152,6 +1366,12 @@
 </t>
         </is>
       </c>
+      <c r="E36" t="n">
+        <v>40</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1172,6 +1392,12 @@
 </t>
         </is>
       </c>
+      <c r="E37" t="n">
+        <v>40</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1192,6 +1418,12 @@
 </t>
         </is>
       </c>
+      <c r="E38" t="n">
+        <v>40</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.5350711345672607</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1212,6 +1444,12 @@
 </t>
         </is>
       </c>
+      <c r="E39" t="n">
+        <v>40</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.4114404618740082</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1232,6 +1470,12 @@
 </t>
         </is>
       </c>
+      <c r="E40" t="n">
+        <v>40</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.4114404618740082</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1252,6 +1496,12 @@
 </t>
         </is>
       </c>
+      <c r="E41" t="n">
+        <v>40</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.5032179951667786</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1272,6 +1522,12 @@
 </t>
         </is>
       </c>
+      <c r="E42" t="n">
+        <v>40</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.5032179951667786</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1292,6 +1548,12 @@
 </t>
         </is>
       </c>
+      <c r="E43" t="n">
+        <v>40</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.5032179951667786</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1312,6 +1574,12 @@
 </t>
         </is>
       </c>
+      <c r="E44" t="n">
+        <v>40</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.5032179951667786</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1332,6 +1600,12 @@
 </t>
         </is>
       </c>
+      <c r="E45" t="n">
+        <v>40</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.5032179951667786</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1352,6 +1626,12 @@
 </t>
         </is>
       </c>
+      <c r="E46" t="n">
+        <v>40</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.5032179951667786</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1372,6 +1652,12 @@
 </t>
         </is>
       </c>
+      <c r="E47" t="n">
+        <v>40</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.5032179951667786</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1390,6 +1676,12 @@
           <t xml:space="preserve"> Local regulatory impacts (in line with OEM future portfolio) including market tailored 
 product &amp; features input.</t>
         </is>
+      </c>
+      <c r="E48" t="n">
+        <v>40</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.4224454164505005</v>
       </c>
     </row>
     <row r="49">
@@ -1414,6 +1706,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E49" t="n">
+        <v>20</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1437,6 +1735,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E50" t="n">
+        <v>20</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1460,6 +1764,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E51" t="n">
+        <v>20</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1483,6 +1793,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E52" t="n">
+        <v>20</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1506,6 +1822,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E53" t="n">
+        <v>20</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1529,6 +1851,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E54" t="n">
+        <v>20</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1552,6 +1880,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E55" t="n">
+        <v>20</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1575,6 +1909,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E56" t="n">
+        <v>20</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1598,6 +1938,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E57" t="n">
+        <v>20</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1621,6 +1967,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E58" t="n">
+        <v>20</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1644,6 +1996,12 @@
 vehicles</t>
         </is>
       </c>
+      <c r="E59" t="n">
+        <v>20</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.6599290370941162</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1664,6 +2022,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E60" t="n">
+        <v>5</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1684,6 +2048,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E61" t="n">
+        <v>5</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1704,6 +2074,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E62" t="n">
+        <v>5</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1724,6 +2100,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E63" t="n">
+        <v>5</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1744,6 +2126,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E64" t="n">
+        <v>5</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1764,6 +2152,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E65" t="n">
+        <v>5</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1784,6 +2178,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E66" t="n">
+        <v>5</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1804,6 +2204,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E67" t="n">
+        <v>5</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1824,6 +2230,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E68" t="n">
+        <v>5</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1844,6 +2256,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E69" t="n">
+        <v>5</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1864,6 +2282,12 @@
 interdependency by 2025</t>
         </is>
       </c>
+      <c r="E70" t="n">
+        <v>5</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.4740377962589264</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -1884,6 +2308,12 @@
 </t>
         </is>
       </c>
+      <c r="E71" t="n">
+        <v>30</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.4175359904766083</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1904,6 +2334,12 @@
 </t>
         </is>
       </c>
+      <c r="E72" t="n">
+        <v>30</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.4175359904766083</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1924,6 +2360,12 @@
 </t>
         </is>
       </c>
+      <c r="E73" t="n">
+        <v>30</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.4175359904766083</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -1943,6 +2385,12 @@
 </t>
         </is>
       </c>
+      <c r="E74" t="n">
+        <v>30</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.4401599764823914</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -1963,6 +2411,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E75" t="n">
+        <v>5</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -1983,6 +2437,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E76" t="n">
+        <v>5</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2003,6 +2463,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E77" t="n">
+        <v>5</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2023,6 +2489,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E78" t="n">
+        <v>5</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2043,6 +2515,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E79" t="n">
+        <v>5</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2063,6 +2541,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E80" t="n">
+        <v>5</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2083,6 +2567,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E81" t="n">
+        <v>5</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2103,6 +2593,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E82" t="n">
+        <v>5</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2123,6 +2619,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E83" t="n">
+        <v>5</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2143,6 +2645,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E84" t="n">
+        <v>5</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2163,6 +2671,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E85" t="n">
+        <v>5</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2183,6 +2697,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E86" t="n">
+        <v>5</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2203,6 +2723,12 @@
 meet local demand.</t>
         </is>
       </c>
+      <c r="E87" t="n">
+        <v>5</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.5501365065574646</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2222,6 +2748,12 @@
 special vehicle offerings to tailor products and assist with tactical sales actions to 
 meet local demand.</t>
         </is>
+      </c>
+      <c r="E88" t="n">
+        <v>5</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.5501365065574646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>